<commit_message>
Adds data and removes readme
</commit_message>
<xml_diff>
--- a/python_analysis/data/1QB/1QBRankings_August25.xlsx
+++ b/python_analysis/data/1QB/1QBRankings_August25.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjzachariason/Dropbox/Late-Round Fantasy Football/_Shared Drive/Patreon/Rankings/Dynasty Rankings/8_2025/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryancontino/Desktop/volatile/python_analysis/data/1QB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7FCA2F-EC07-974F-A127-78374E97AF78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA43C135-ABEC-F548-B11F-F86937778BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="7220" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{8B1390D6-95F4-C24A-B3AF-0CA9228166C8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" xr2:uid="{8B1390D6-95F4-C24A-B3AF-0CA9228166C8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Read Me" sheetId="2" r:id="rId1"/>
-    <sheet name="Rankings and Tiers" sheetId="1" r:id="rId2"/>
+    <sheet name="Rankings and Tiers" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Rankings and Tiers'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Rankings and Tiers'!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="210">
   <si>
     <t>Overall</t>
   </si>
@@ -240,12 +239,6 @@
   </si>
   <si>
     <t>David Njoku</t>
-  </si>
-  <si>
-    <t>By viewing this digital product, you agree that under no circumstances shall you use this digital product or any portion of this digital product for anything but your own personal use and reference. For the avoidance of doubt, you shall not copy, re-sell, sublicense, rent out, share or otherwise distribute this digital product, or any other Late-Round Fantasy Football digital product, whether modified or not, to any third party. You agree not to use any derivative of Late-Round Fantasy Football’s products in a way which might be detrimental to Late-Round Fantasy Football or damage Late-Round Fantasy Football’s reputation.</t>
-  </si>
-  <si>
-    <t>Terms</t>
   </si>
   <si>
     <t>Breece Hall</t>
@@ -684,55 +677,23 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFCEE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -740,60 +701,18 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1107,90 +1026,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5DB6E3E-D5DA-BE40-9DC0-94C04F4A8891}">
-  <dimension ref="B2:C19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11" style="2"/>
-    <col min="2" max="2" width="47.796875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="78" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="11" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:3" ht="23" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" ht="101" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="8"/>
-    </row>
-    <row r="7" spans="2:3" ht="23" x14ac:dyDescent="0.25">
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="4"/>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="4"/>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="4"/>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B12" s="4"/>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="4"/>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="4"/>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B15" s="4"/>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="4"/>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17" s="4"/>
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="4"/>
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="4"/>
-      <c r="C19" s="3"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B7:C7"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E79AA84A-6624-1E4A-A0A6-C46EEDC7685B}">
   <dimension ref="A1:F201"/>
   <sheetViews>
@@ -1205,7 +1040,7 @@
     <col min="3" max="3" width="11.59765625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.796875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" style="6"/>
+    <col min="6" max="6" width="11" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
@@ -1224,8 +1059,8 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>121</v>
+      <c r="F1" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
@@ -1236,7 +1071,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -1244,7 +1079,7 @@
       <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="2">
         <v>25.416666666666668</v>
       </c>
     </row>
@@ -1256,7 +1091,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D3" s="1">
         <v>2</v>
@@ -1264,7 +1099,7 @@
       <c r="E3" s="1">
         <v>1</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="2">
         <v>26.125</v>
       </c>
     </row>
@@ -1273,10 +1108,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D4" s="1">
         <v>3</v>
@@ -1284,7 +1119,7 @@
       <c r="E4" s="1">
         <v>2</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="2">
         <v>22.008333333333333</v>
       </c>
     </row>
@@ -1293,10 +1128,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
@@ -1304,7 +1139,7 @@
       <c r="E5" s="1">
         <v>2</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="2">
         <v>23.502777777777776</v>
       </c>
     </row>
@@ -1313,10 +1148,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D6" s="1">
         <v>2</v>
@@ -1324,7 +1159,7 @@
       <c r="E6" s="1">
         <v>2</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="2">
         <v>23.363888888888887</v>
       </c>
     </row>
@@ -1333,10 +1168,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D7" s="1">
         <v>3</v>
@@ -1344,7 +1179,7 @@
       <c r="E7" s="1">
         <v>2</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="2">
         <v>21.661111111111111</v>
       </c>
     </row>
@@ -1353,10 +1188,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
@@ -1364,7 +1199,7 @@
       <c r="E8" s="1">
         <v>2</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="2">
         <v>22.633333333333333</v>
       </c>
     </row>
@@ -1376,7 +1211,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D9" s="1">
         <v>4</v>
@@ -1384,7 +1219,7 @@
       <c r="E9" s="1">
         <v>2</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="2">
         <v>26.31388888888889</v>
       </c>
     </row>
@@ -1393,10 +1228,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D10" s="1">
         <v>5</v>
@@ -1404,7 +1239,7 @@
       <c r="E10" s="1">
         <v>2</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="2">
         <v>24.172222222222221</v>
       </c>
     </row>
@@ -1413,10 +1248,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D11" s="1">
         <v>6</v>
@@ -1424,7 +1259,7 @@
       <c r="E11" s="1">
         <v>2</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="2">
         <v>22.81388888888889</v>
       </c>
     </row>
@@ -1436,7 +1271,7 @@
         <v>45</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D12" s="1">
         <v>7</v>
@@ -1444,7 +1279,7 @@
       <c r="E12" s="1">
         <v>2</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="2">
         <v>25.769444444444446</v>
       </c>
     </row>
@@ -1453,10 +1288,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D13" s="1">
         <v>8</v>
@@ -1464,7 +1299,7 @@
       <c r="E13" s="1">
         <v>3</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="2">
         <v>24.019444444444446</v>
       </c>
     </row>
@@ -1476,7 +1311,7 @@
         <v>63</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D14" s="1">
         <v>9</v>
@@ -1484,7 +1319,7 @@
       <c r="E14" s="1">
         <v>3</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="2">
         <v>26.366666666666667</v>
       </c>
     </row>
@@ -1493,10 +1328,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D15" s="1">
         <v>10</v>
@@ -1504,7 +1339,7 @@
       <c r="E15" s="1">
         <v>3</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="2">
         <v>23.722222222222221</v>
       </c>
     </row>
@@ -1516,7 +1351,7 @@
         <v>41</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
@@ -1524,7 +1359,7 @@
       <c r="E16" s="1">
         <v>3</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="2">
         <v>29.194444444444443</v>
       </c>
     </row>
@@ -1533,10 +1368,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D17" s="1">
         <v>11</v>
@@ -1544,7 +1379,7 @@
       <c r="E17" s="1">
         <v>3</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="2">
         <v>23.463888888888889</v>
       </c>
     </row>
@@ -1553,10 +1388,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D18" s="1">
         <v>2</v>
@@ -1564,7 +1399,7 @@
       <c r="E18" s="1">
         <v>3</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="2">
         <v>24.619444444444444</v>
       </c>
     </row>
@@ -1576,7 +1411,7 @@
         <v>48</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D19" s="1">
         <v>3</v>
@@ -1584,7 +1419,7 @@
       <c r="E19" s="1">
         <v>3</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="2">
         <v>28.566666666666666</v>
       </c>
     </row>
@@ -1593,10 +1428,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D20" s="1">
         <v>4</v>
@@ -1604,7 +1439,7 @@
       <c r="E20" s="1">
         <v>4</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="2">
         <v>22.375</v>
       </c>
     </row>
@@ -1613,10 +1448,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D21" s="1">
         <v>12</v>
@@ -1624,7 +1459,7 @@
       <c r="E21" s="1">
         <v>4</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="2">
         <v>22.972222222222221</v>
       </c>
     </row>
@@ -1633,10 +1468,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D22" s="1">
         <v>13</v>
@@ -1644,7 +1479,7 @@
       <c r="E22" s="1">
         <v>4</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="2">
         <v>22.322222222222223</v>
       </c>
     </row>
@@ -1653,10 +1488,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D23" s="1">
         <v>2</v>
@@ -1664,7 +1499,7 @@
       <c r="E23" s="1">
         <v>4</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="2">
         <v>25.691666666666666</v>
       </c>
     </row>
@@ -1673,10 +1508,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D24" s="1">
         <v>5</v>
@@ -1684,7 +1519,7 @@
       <c r="E24" s="1">
         <v>4</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="2">
         <v>23.8</v>
       </c>
     </row>
@@ -1696,7 +1531,7 @@
         <v>25</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D25" s="1">
         <v>6</v>
@@ -1704,7 +1539,7 @@
       <c r="E25" s="1">
         <v>4</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="2">
         <v>28.483333333333334</v>
       </c>
     </row>
@@ -1713,10 +1548,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D26" s="1">
         <v>7</v>
@@ -1724,7 +1559,7 @@
       <c r="E26" s="1">
         <v>5</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="2">
         <v>22.866666666666667</v>
       </c>
     </row>
@@ -1733,10 +1568,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D27" s="1">
         <v>14</v>
@@ -1744,7 +1579,7 @@
       <c r="E27" s="1">
         <v>5</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="2">
         <v>22.202777777777779</v>
       </c>
     </row>
@@ -1753,10 +1588,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D28" s="1">
         <v>15</v>
@@ -1764,7 +1599,7 @@
       <c r="E28" s="1">
         <v>5</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F28" s="2">
         <v>25.024999999999999</v>
       </c>
     </row>
@@ -1776,7 +1611,7 @@
         <v>8</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D29" s="1">
         <v>16</v>
@@ -1784,7 +1619,7 @@
       <c r="E29" s="1">
         <v>5</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F29" s="2">
         <v>28.086111111111112</v>
       </c>
     </row>
@@ -1793,10 +1628,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D30" s="1">
         <v>8</v>
@@ -1804,7 +1639,7 @@
       <c r="E30" s="1">
         <v>6</v>
       </c>
-      <c r="F30" s="6">
+      <c r="F30" s="2">
         <v>22.774999999999999</v>
       </c>
     </row>
@@ -1813,10 +1648,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D31" s="1">
         <v>9</v>
@@ -1824,7 +1659,7 @@
       <c r="E31" s="1">
         <v>6</v>
       </c>
-      <c r="F31" s="6">
+      <c r="F31" s="2">
         <v>24.169444444444444</v>
       </c>
     </row>
@@ -1836,7 +1671,7 @@
         <v>7</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D32" s="1">
         <v>10</v>
@@ -1844,7 +1679,7 @@
       <c r="E32" s="1">
         <v>6</v>
       </c>
-      <c r="F32" s="6">
+      <c r="F32" s="2">
         <v>26.533333333333335</v>
       </c>
     </row>
@@ -1856,7 +1691,7 @@
         <v>23</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D33" s="1">
         <v>17</v>
@@ -1864,7 +1699,7 @@
       <c r="E33" s="1">
         <v>6</v>
       </c>
-      <c r="F33" s="6">
+      <c r="F33" s="2">
         <v>26.536111111111111</v>
       </c>
     </row>
@@ -1876,7 +1711,7 @@
         <v>62</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D34" s="1">
         <v>4</v>
@@ -1884,7 +1719,7 @@
       <c r="E34" s="1">
         <v>7</v>
       </c>
-      <c r="F34" s="6">
+      <c r="F34" s="2">
         <v>26.983333333333334</v>
       </c>
     </row>
@@ -1893,10 +1728,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D35" s="1">
         <v>3</v>
@@ -1904,7 +1739,7 @@
       <c r="E35" s="1">
         <v>7</v>
       </c>
-      <c r="F35" s="6">
+      <c r="F35" s="2">
         <v>24.552777777777777</v>
       </c>
     </row>
@@ -1913,10 +1748,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D36" s="1">
         <v>18</v>
@@ -1924,7 +1759,7 @@
       <c r="E36" s="1">
         <v>7</v>
       </c>
-      <c r="F36" s="6">
+      <c r="F36" s="2">
         <v>22.797222222222221</v>
       </c>
     </row>
@@ -1933,10 +1768,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D37" s="1">
         <v>11</v>
@@ -1944,7 +1779,7 @@
       <c r="E37" s="1">
         <v>7</v>
       </c>
-      <c r="F37" s="6">
+      <c r="F37" s="2">
         <v>24.780555555555555</v>
       </c>
     </row>
@@ -1953,10 +1788,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D38" s="1">
         <v>19</v>
@@ -1964,7 +1799,7 @@
       <c r="E38" s="1">
         <v>7</v>
       </c>
-      <c r="F38" s="6">
+      <c r="F38" s="2">
         <v>25.274999999999999</v>
       </c>
     </row>
@@ -1976,7 +1811,7 @@
         <v>32</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D39" s="1">
         <v>20</v>
@@ -1984,7 +1819,7 @@
       <c r="E39" s="1">
         <v>7</v>
       </c>
-      <c r="F39" s="6">
+      <c r="F39" s="2">
         <v>26.713888888888889</v>
       </c>
     </row>
@@ -1996,7 +1831,7 @@
         <v>51</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D40" s="1">
         <v>5</v>
@@ -2004,7 +1839,7 @@
       <c r="E40" s="1">
         <v>8</v>
       </c>
-      <c r="F40" s="6">
+      <c r="F40" s="2">
         <v>28.641666666666666</v>
       </c>
     </row>
@@ -2013,10 +1848,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D41" s="1">
         <v>21</v>
@@ -2024,7 +1859,7 @@
       <c r="E41" s="1">
         <v>8</v>
       </c>
-      <c r="F41" s="6">
+      <c r="F41" s="2">
         <v>23.161111111111111</v>
       </c>
     </row>
@@ -2033,10 +1868,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D42" s="1">
         <v>12</v>
@@ -2044,7 +1879,7 @@
       <c r="E42" s="1">
         <v>8</v>
       </c>
-      <c r="F42" s="6">
+      <c r="F42" s="2">
         <v>25.361111111111111</v>
       </c>
     </row>
@@ -2053,10 +1888,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D43" s="1">
         <v>22</v>
@@ -2064,7 +1899,7 @@
       <c r="E43" s="1">
         <v>8</v>
       </c>
-      <c r="F43" s="6">
+      <c r="F43" s="2">
         <v>24.888888888888889</v>
       </c>
     </row>
@@ -2073,10 +1908,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D44" s="1">
         <v>23</v>
@@ -2084,7 +1919,7 @@
       <c r="E44" s="1">
         <v>8</v>
       </c>
-      <c r="F44" s="6">
+      <c r="F44" s="2">
         <v>23.511111111111113</v>
       </c>
     </row>
@@ -2093,10 +1928,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D45" s="1">
         <v>13</v>
@@ -2104,7 +1939,7 @@
       <c r="E45" s="1">
         <v>8</v>
       </c>
-      <c r="F45" s="6">
+      <c r="F45" s="2">
         <v>25.85</v>
       </c>
     </row>
@@ -2113,10 +1948,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D46" s="1">
         <v>14</v>
@@ -2124,7 +1959,7 @@
       <c r="E46" s="1">
         <v>9</v>
       </c>
-      <c r="F46" s="6">
+      <c r="F46" s="2">
         <v>24.930555555555557</v>
       </c>
     </row>
@@ -2136,7 +1971,7 @@
         <v>17</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D47" s="1">
         <v>24</v>
@@ -2144,7 +1979,7 @@
       <c r="E47" s="1">
         <v>9</v>
       </c>
-      <c r="F47" s="6">
+      <c r="F47" s="2">
         <v>26.683333333333334</v>
       </c>
     </row>
@@ -2156,7 +1991,7 @@
         <v>43</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D48" s="1">
         <v>15</v>
@@ -2164,7 +1999,7 @@
       <c r="E48" s="1">
         <v>9</v>
       </c>
-      <c r="F48" s="6">
+      <c r="F48" s="2">
         <v>27.472222222222221</v>
       </c>
     </row>
@@ -2173,10 +2008,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D49" s="1">
         <v>25</v>
@@ -2184,7 +2019,7 @@
       <c r="E49" s="1">
         <v>10</v>
       </c>
-      <c r="F49" s="6">
+      <c r="F49" s="2">
         <v>22.261111111111113</v>
       </c>
     </row>
@@ -2193,10 +2028,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D50" s="1">
         <v>26</v>
@@ -2204,7 +2039,7 @@
       <c r="E50" s="1">
         <v>10</v>
       </c>
-      <c r="F50" s="6">
+      <c r="F50" s="2">
         <v>24.347222222222221</v>
       </c>
     </row>
@@ -2213,10 +2048,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D51" s="1">
         <v>27</v>
@@ -2224,7 +2059,7 @@
       <c r="E51" s="1">
         <v>10</v>
       </c>
-      <c r="F51" s="6">
+      <c r="F51" s="2">
         <v>25.094444444444445</v>
       </c>
     </row>
@@ -2236,7 +2071,7 @@
         <v>9</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D52" s="1">
         <v>28</v>
@@ -2244,7 +2079,7 @@
       <c r="E52" s="1">
         <v>10</v>
       </c>
-      <c r="F52" s="6">
+      <c r="F52" s="2">
         <v>27.630555555555556</v>
       </c>
     </row>
@@ -2256,7 +2091,7 @@
         <v>15</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D53" s="1">
         <v>16</v>
@@ -2264,7 +2099,7 @@
       <c r="E53" s="1">
         <v>10</v>
       </c>
-      <c r="F53" s="6">
+      <c r="F53" s="2">
         <v>29.15</v>
       </c>
     </row>
@@ -2273,10 +2108,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D54" s="1">
         <v>29</v>
@@ -2284,7 +2119,7 @@
       <c r="E54" s="1">
         <v>10</v>
       </c>
-      <c r="F54" s="6">
+      <c r="F54" s="2">
         <v>24.408333333333335</v>
       </c>
     </row>
@@ -2293,10 +2128,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D55" s="1">
         <v>30</v>
@@ -2304,7 +2139,7 @@
       <c r="E55" s="1">
         <v>11</v>
       </c>
-      <c r="F55" s="6">
+      <c r="F55" s="2">
         <v>22</v>
       </c>
     </row>
@@ -2313,10 +2148,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D56" s="1">
         <v>17</v>
@@ -2324,7 +2159,7 @@
       <c r="E56" s="1">
         <v>11</v>
       </c>
-      <c r="F56" s="6">
+      <c r="F56" s="2">
         <v>24.491666666666667</v>
       </c>
     </row>
@@ -2336,7 +2171,7 @@
         <v>37</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D57" s="1">
         <v>6</v>
@@ -2344,7 +2179,7 @@
       <c r="E57" s="1">
         <v>11</v>
       </c>
-      <c r="F57" s="6">
+      <c r="F57" s="2">
         <v>29.872222222222224</v>
       </c>
     </row>
@@ -2356,7 +2191,7 @@
         <v>27</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D58" s="1">
         <v>18</v>
@@ -2364,7 +2199,7 @@
       <c r="E58" s="1">
         <v>11</v>
       </c>
-      <c r="F58" s="6">
+      <c r="F58" s="2">
         <v>31.574999999999999</v>
       </c>
     </row>
@@ -2373,10 +2208,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D59" s="1">
         <v>19</v>
@@ -2384,7 +2219,7 @@
       <c r="E59" s="1">
         <v>11</v>
       </c>
-      <c r="F59" s="6">
+      <c r="F59" s="2">
         <v>21.963888888888889</v>
       </c>
     </row>
@@ -2393,10 +2228,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D60" s="1">
         <v>31</v>
@@ -2404,7 +2239,7 @@
       <c r="E60" s="1">
         <v>11</v>
       </c>
-      <c r="F60" s="6">
+      <c r="F60" s="2">
         <v>21.636111111111113</v>
       </c>
     </row>
@@ -2416,7 +2251,7 @@
         <v>28</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D61" s="1">
         <v>32</v>
@@ -2424,7 +2259,7 @@
       <c r="E61" s="1">
         <v>12</v>
       </c>
-      <c r="F61" s="6">
+      <c r="F61" s="2">
         <v>29.877777777777776</v>
       </c>
     </row>
@@ -2436,7 +2271,7 @@
         <v>29</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D62" s="1">
         <v>33</v>
@@ -2444,7 +2279,7 @@
       <c r="E62" s="1">
         <v>12</v>
       </c>
-      <c r="F62" s="6">
+      <c r="F62" s="2">
         <v>28.297222222222221</v>
       </c>
     </row>
@@ -2453,10 +2288,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D63" s="1">
         <v>34</v>
@@ -2464,7 +2299,7 @@
       <c r="E63" s="1">
         <v>13</v>
       </c>
-      <c r="F63" s="6">
+      <c r="F63" s="2">
         <v>24.894444444444446</v>
       </c>
     </row>
@@ -2476,7 +2311,7 @@
         <v>39</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D64" s="1">
         <v>35</v>
@@ -2484,7 +2319,7 @@
       <c r="E64" s="1">
         <v>13</v>
       </c>
-      <c r="F64" s="6">
+      <c r="F64" s="2">
         <v>27.372222222222224</v>
       </c>
     </row>
@@ -2496,7 +2331,7 @@
         <v>49</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D65" s="1">
         <v>7</v>
@@ -2504,7 +2339,7 @@
       <c r="E65" s="1">
         <v>13</v>
       </c>
-      <c r="F65" s="6">
+      <c r="F65" s="2">
         <v>27.391666666666666</v>
       </c>
     </row>
@@ -2516,7 +2351,7 @@
         <v>35</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D66" s="1">
         <v>4</v>
@@ -2524,7 +2359,7 @@
       <c r="E66" s="1">
         <v>13</v>
       </c>
-      <c r="F66" s="6">
+      <c r="F66" s="2">
         <v>31.81111111111111</v>
       </c>
     </row>
@@ -2533,10 +2368,10 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D67" s="1">
         <v>36</v>
@@ -2544,7 +2379,7 @@
       <c r="E67" s="1">
         <v>13</v>
       </c>
-      <c r="F67" s="6">
+      <c r="F67" s="2">
         <v>23.969444444444445</v>
       </c>
     </row>
@@ -2553,10 +2388,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D68" s="1">
         <v>8</v>
@@ -2564,7 +2399,7 @@
       <c r="E68" s="1">
         <v>13</v>
       </c>
-      <c r="F68" s="6">
+      <c r="F68" s="2">
         <v>22.919444444444444</v>
       </c>
     </row>
@@ -2573,10 +2408,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D69" s="1">
         <v>9</v>
@@ -2584,7 +2419,7 @@
       <c r="E69" s="1">
         <v>13</v>
       </c>
-      <c r="F69" s="6">
+      <c r="F69" s="2">
         <v>23.702777777777779</v>
       </c>
     </row>
@@ -2593,10 +2428,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D70" s="1">
         <v>5</v>
@@ -2604,7 +2439,7 @@
       <c r="E70" s="1">
         <v>13</v>
       </c>
-      <c r="F70" s="6">
+      <c r="F70" s="2">
         <v>21.31111111111111</v>
       </c>
     </row>
@@ -2613,10 +2448,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D71" s="1">
         <v>10</v>
@@ -2624,7 +2459,7 @@
       <c r="E71" s="1">
         <v>13</v>
       </c>
-      <c r="F71" s="6">
+      <c r="F71" s="2">
         <v>25.433333333333334</v>
       </c>
     </row>
@@ -2633,10 +2468,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D72" s="1">
         <v>6</v>
@@ -2644,7 +2479,7 @@
       <c r="E72" s="1">
         <v>13</v>
       </c>
-      <c r="F72" s="6">
+      <c r="F72" s="2">
         <v>23.18611111111111</v>
       </c>
     </row>
@@ -2653,10 +2488,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D73" s="1">
         <v>37</v>
@@ -2664,7 +2499,7 @@
       <c r="E73" s="1">
         <v>13</v>
       </c>
-      <c r="F73" s="6">
+      <c r="F73" s="2">
         <v>25.494444444444444</v>
       </c>
     </row>
@@ -2676,7 +2511,7 @@
         <v>16</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D74" s="1">
         <v>38</v>
@@ -2684,7 +2519,7 @@
       <c r="E74" s="1">
         <v>13</v>
       </c>
-      <c r="F74" s="6">
+      <c r="F74" s="2">
         <v>32.602777777777774</v>
       </c>
     </row>
@@ -2693,10 +2528,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D75" s="1">
         <v>39</v>
@@ -2704,7 +2539,7 @@
       <c r="E75" s="1">
         <v>14</v>
       </c>
-      <c r="F75" s="6">
+      <c r="F75" s="2">
         <v>22.627777777777776</v>
       </c>
     </row>
@@ -2713,10 +2548,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D76" s="1">
         <v>40</v>
@@ -2724,7 +2559,7 @@
       <c r="E76" s="1">
         <v>14</v>
       </c>
-      <c r="F76" s="6">
+      <c r="F76" s="2">
         <v>25.258333333333333</v>
       </c>
     </row>
@@ -2733,10 +2568,10 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D77" s="1">
         <v>41</v>
@@ -2744,7 +2579,7 @@
       <c r="E77" s="1">
         <v>14</v>
       </c>
-      <c r="F77" s="6">
+      <c r="F77" s="2">
         <v>23.419444444444444</v>
       </c>
     </row>
@@ -2753,10 +2588,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D78" s="1">
         <v>11</v>
@@ -2764,7 +2599,7 @@
       <c r="E78" s="1">
         <v>14</v>
       </c>
-      <c r="F78" s="6">
+      <c r="F78" s="2">
         <v>23.827777777777779</v>
       </c>
     </row>
@@ -2773,10 +2608,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D79" s="1">
         <v>20</v>
@@ -2784,7 +2619,7 @@
       <c r="E79" s="1">
         <v>14</v>
       </c>
-      <c r="F79" s="6">
+      <c r="F79" s="2">
         <v>21.672222222222221</v>
       </c>
     </row>
@@ -2796,7 +2631,7 @@
         <v>36</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D80" s="1">
         <v>42</v>
@@ -2804,7 +2639,7 @@
       <c r="E80" s="1">
         <v>14</v>
       </c>
-      <c r="F80" s="6">
+      <c r="F80" s="2">
         <v>26.269444444444446</v>
       </c>
     </row>
@@ -2816,7 +2651,7 @@
         <v>10</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D81" s="1">
         <v>43</v>
@@ -2824,7 +2659,7 @@
       <c r="E81" s="1">
         <v>14</v>
       </c>
-      <c r="F81" s="6">
+      <c r="F81" s="2">
         <v>31.416666666666668</v>
       </c>
     </row>
@@ -2833,10 +2668,10 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D82" s="1">
         <v>21</v>
@@ -2844,7 +2679,7 @@
       <c r="E82" s="1">
         <v>14</v>
       </c>
-      <c r="F82" s="6">
+      <c r="F82" s="2">
         <v>26.138888888888889</v>
       </c>
     </row>
@@ -2856,7 +2691,7 @@
         <v>31</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D83" s="1">
         <v>44</v>
@@ -2864,7 +2699,7 @@
       <c r="E83" s="1">
         <v>14</v>
       </c>
-      <c r="F83" s="6">
+      <c r="F83" s="2">
         <v>31.944444444444443</v>
       </c>
     </row>
@@ -2876,7 +2711,7 @@
         <v>21</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D84" s="1">
         <v>45</v>
@@ -2884,7 +2719,7 @@
       <c r="E84" s="1">
         <v>14</v>
       </c>
-      <c r="F84" s="6">
+      <c r="F84" s="2">
         <v>29.427777777777777</v>
       </c>
     </row>
@@ -2896,7 +2731,7 @@
         <v>50</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D85" s="1">
         <v>46</v>
@@ -2904,7 +2739,7 @@
       <c r="E85" s="1">
         <v>15</v>
       </c>
-      <c r="F85" s="6">
+      <c r="F85" s="2">
         <v>29.808333333333334</v>
       </c>
     </row>
@@ -2913,10 +2748,10 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D86" s="1">
         <v>47</v>
@@ -2924,7 +2759,7 @@
       <c r="E86" s="1">
         <v>15</v>
       </c>
-      <c r="F86" s="6">
+      <c r="F86" s="2">
         <v>22.205555555555556</v>
       </c>
     </row>
@@ -2936,7 +2771,7 @@
         <v>60</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D87" s="1">
         <v>48</v>
@@ -2944,7 +2779,7 @@
       <c r="E87" s="1">
         <v>15</v>
       </c>
-      <c r="F87" s="6">
+      <c r="F87" s="2">
         <v>28.727777777777778</v>
       </c>
     </row>
@@ -2956,7 +2791,7 @@
         <v>40</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D88" s="1">
         <v>7</v>
@@ -2964,7 +2799,7 @@
       <c r="E88" s="1">
         <v>15</v>
       </c>
-      <c r="F88" s="6">
+      <c r="F88" s="2">
         <v>28.077777777777779</v>
       </c>
     </row>
@@ -2976,7 +2811,7 @@
         <v>26</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D89" s="1">
         <v>22</v>
@@ -2984,7 +2819,7 @@
       <c r="E89" s="1">
         <v>15</v>
       </c>
-      <c r="F89" s="6">
+      <c r="F89" s="2">
         <v>30.016666666666666</v>
       </c>
     </row>
@@ -2993,10 +2828,10 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D90" s="1">
         <v>8</v>
@@ -3004,7 +2839,7 @@
       <c r="E90" s="1">
         <v>15</v>
       </c>
-      <c r="F90" s="6">
+      <c r="F90" s="2">
         <v>24.744444444444444</v>
       </c>
     </row>
@@ -3016,7 +2851,7 @@
         <v>34</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D91" s="1">
         <v>49</v>
@@ -3024,7 +2859,7 @@
       <c r="E91" s="1">
         <v>15</v>
       </c>
-      <c r="F91" s="6">
+      <c r="F91" s="2">
         <v>27.822222222222223</v>
       </c>
     </row>
@@ -3036,7 +2871,7 @@
         <v>42</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D92" s="1">
         <v>23</v>
@@ -3044,7 +2879,7 @@
       <c r="E92" s="1">
         <v>15</v>
       </c>
-      <c r="F92" s="6">
+      <c r="F92" s="2">
         <v>28.15</v>
       </c>
     </row>
@@ -3056,7 +2891,7 @@
         <v>47</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D93" s="1">
         <v>12</v>
@@ -3064,7 +2899,7 @@
       <c r="E93" s="1">
         <v>15</v>
       </c>
-      <c r="F93" s="6">
+      <c r="F93" s="2">
         <v>27.9</v>
       </c>
     </row>
@@ -3073,10 +2908,10 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D94" s="1">
         <v>50</v>
@@ -3084,7 +2919,7 @@
       <c r="E94" s="1">
         <v>16</v>
       </c>
-      <c r="F94" s="6">
+      <c r="F94" s="2">
         <v>26.919444444444444</v>
       </c>
     </row>
@@ -3093,10 +2928,10 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D95" s="1">
         <v>13</v>
@@ -3104,7 +2939,7 @@
       <c r="E95" s="1">
         <v>16</v>
       </c>
-      <c r="F95" s="6">
+      <c r="F95" s="2">
         <v>25.594444444444445</v>
       </c>
     </row>
@@ -3116,7 +2951,7 @@
         <v>33</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D96" s="1">
         <v>51</v>
@@ -3124,7 +2959,7 @@
       <c r="E96" s="1">
         <v>16</v>
       </c>
-      <c r="F96" s="6">
+      <c r="F96" s="2">
         <v>30.613888888888887</v>
       </c>
     </row>
@@ -3133,10 +2968,10 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D97" s="1">
         <v>14</v>
@@ -3144,7 +2979,7 @@
       <c r="E97" s="1">
         <v>16</v>
       </c>
-      <c r="F97" s="6">
+      <c r="F97" s="2">
         <v>30.297222222222221</v>
       </c>
     </row>
@@ -3153,10 +2988,10 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D98" s="1">
         <v>15</v>
@@ -3164,7 +2999,7 @@
       <c r="E98" s="1">
         <v>16</v>
       </c>
-      <c r="F98" s="6">
+      <c r="F98" s="2">
         <v>26.747222222222224</v>
       </c>
     </row>
@@ -3173,10 +3008,10 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D99" s="1">
         <v>24</v>
@@ -3184,7 +3019,7 @@
       <c r="E99" s="1">
         <v>16</v>
       </c>
-      <c r="F99" s="6">
+      <c r="F99" s="2">
         <v>25.413888888888888</v>
       </c>
     </row>
@@ -3193,10 +3028,10 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D100" s="1">
         <v>16</v>
@@ -3204,7 +3039,7 @@
       <c r="E100" s="1">
         <v>17</v>
       </c>
-      <c r="F100" s="6">
+      <c r="F100" s="2">
         <v>22.530555555555555</v>
       </c>
     </row>
@@ -3213,10 +3048,10 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D101" s="1">
         <v>25</v>
@@ -3224,7 +3059,7 @@
       <c r="E101" s="1">
         <v>17</v>
       </c>
-      <c r="F101" s="6">
+      <c r="F101" s="2">
         <v>24.56388888888889</v>
       </c>
     </row>
@@ -3236,7 +3071,7 @@
         <v>24</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D102" s="1">
         <v>26</v>
@@ -3244,7 +3079,7 @@
       <c r="E102" s="1">
         <v>17</v>
       </c>
-      <c r="F102" s="6">
+      <c r="F102" s="2">
         <v>29.019444444444446</v>
       </c>
     </row>
@@ -3253,10 +3088,10 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D103" s="1">
         <v>17</v>
@@ -3264,7 +3099,7 @@
       <c r="E103" s="1">
         <v>17</v>
       </c>
-      <c r="F103" s="6">
+      <c r="F103" s="2">
         <v>23.183333333333334</v>
       </c>
     </row>
@@ -3273,10 +3108,10 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D104" s="1">
         <v>9</v>
@@ -3284,7 +3119,7 @@
       <c r="E104" s="1">
         <v>17</v>
       </c>
-      <c r="F104" s="6">
+      <c r="F104" s="2">
         <v>25.786111111111111</v>
       </c>
     </row>
@@ -3296,7 +3131,7 @@
         <v>19</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D105" s="1">
         <v>27</v>
@@ -3304,7 +3139,7 @@
       <c r="E105" s="1">
         <v>17</v>
       </c>
-      <c r="F105" s="6">
+      <c r="F105" s="2">
         <v>26.547222222222221</v>
       </c>
     </row>
@@ -3313,10 +3148,10 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D106" s="1">
         <v>28</v>
@@ -3324,7 +3159,7 @@
       <c r="E106" s="1">
         <v>17</v>
       </c>
-      <c r="F106" s="6">
+      <c r="F106" s="2">
         <v>25.68888888888889</v>
       </c>
     </row>
@@ -3336,7 +3171,7 @@
         <v>53</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D107" s="1">
         <v>52</v>
@@ -3344,7 +3179,7 @@
       <c r="E107" s="1">
         <v>17</v>
       </c>
-      <c r="F107" s="6">
+      <c r="F107" s="2">
         <v>27.755555555555556</v>
       </c>
     </row>
@@ -3356,7 +3191,7 @@
         <v>57</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D108" s="1">
         <v>29</v>
@@ -3364,7 +3199,7 @@
       <c r="E108" s="1">
         <v>17</v>
       </c>
-      <c r="F108" s="6">
+      <c r="F108" s="2">
         <v>30.238888888888887</v>
       </c>
     </row>
@@ -3373,10 +3208,10 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D109" s="1">
         <v>30</v>
@@ -3384,7 +3219,7 @@
       <c r="E109" s="1">
         <v>17</v>
       </c>
-      <c r="F109" s="6">
+      <c r="F109" s="2">
         <v>22.463888888888889</v>
       </c>
     </row>
@@ -3393,10 +3228,10 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D110" s="1">
         <v>31</v>
@@ -3404,7 +3239,7 @@
       <c r="E110" s="1">
         <v>17</v>
       </c>
-      <c r="F110" s="6">
+      <c r="F110" s="2">
         <v>23.488888888888887</v>
       </c>
     </row>
@@ -3413,10 +3248,10 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D111" s="1">
         <v>53</v>
@@ -3424,7 +3259,7 @@
       <c r="E111" s="1">
         <v>17</v>
       </c>
-      <c r="F111" s="6">
+      <c r="F111" s="2">
         <v>23.047222222222221</v>
       </c>
     </row>
@@ -3433,10 +3268,10 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D112" s="1">
         <v>54</v>
@@ -3444,7 +3279,7 @@
       <c r="E112" s="1">
         <v>17</v>
       </c>
-      <c r="F112" s="6">
+      <c r="F112" s="2">
         <v>28.058333333333334</v>
       </c>
     </row>
@@ -3453,10 +3288,10 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D113" s="1">
         <v>55</v>
@@ -3464,7 +3299,7 @@
       <c r="E113" s="1">
         <v>18</v>
       </c>
-      <c r="F113" s="6">
+      <c r="F113" s="2">
         <v>23.366666666666667</v>
       </c>
     </row>
@@ -3473,10 +3308,10 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D114" s="1">
         <v>56</v>
@@ -3484,7 +3319,7 @@
       <c r="E114" s="1">
         <v>18</v>
       </c>
-      <c r="F114" s="6">
+      <c r="F114" s="2">
         <v>22.619444444444444</v>
       </c>
     </row>
@@ -3493,10 +3328,10 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D115" s="1">
         <v>57</v>
@@ -3504,7 +3339,7 @@
       <c r="E115" s="1">
         <v>18</v>
       </c>
-      <c r="F115" s="6">
+      <c r="F115" s="2">
         <v>22.908333333333335</v>
       </c>
     </row>
@@ -3516,7 +3351,7 @@
         <v>12</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D116" s="1">
         <v>58</v>
@@ -3524,7 +3359,7 @@
       <c r="E116" s="1">
         <v>18</v>
       </c>
-      <c r="F116" s="6">
+      <c r="F116" s="2">
         <v>29.544444444444444</v>
       </c>
     </row>
@@ -3533,10 +3368,10 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D117" s="1">
         <v>32</v>
@@ -3544,7 +3379,7 @@
       <c r="E117" s="1">
         <v>18</v>
       </c>
-      <c r="F117" s="6">
+      <c r="F117" s="2">
         <v>26.75</v>
       </c>
     </row>
@@ -3556,7 +3391,7 @@
         <v>56</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D118" s="1">
         <v>33</v>
@@ -3564,7 +3399,7 @@
       <c r="E118" s="1">
         <v>18</v>
       </c>
-      <c r="F118" s="6">
+      <c r="F118" s="2">
         <v>28.252777777777776</v>
       </c>
     </row>
@@ -3576,7 +3411,7 @@
         <v>61</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D119" s="1">
         <v>18</v>
@@ -3584,7 +3419,7 @@
       <c r="E119" s="1">
         <v>19</v>
       </c>
-      <c r="F119" s="6">
+      <c r="F119" s="2">
         <v>25.819444444444443</v>
       </c>
     </row>
@@ -3593,10 +3428,10 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D120" s="1">
         <v>34</v>
@@ -3604,7 +3439,7 @@
       <c r="E120" s="1">
         <v>19</v>
       </c>
-      <c r="F120" s="6">
+      <c r="F120" s="2">
         <v>26.18611111111111</v>
       </c>
     </row>
@@ -3616,7 +3451,7 @@
         <v>22</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D121" s="1">
         <v>59</v>
@@ -3624,7 +3459,7 @@
       <c r="E121" s="1">
         <v>19</v>
       </c>
-      <c r="F121" s="6">
+      <c r="F121" s="2">
         <v>31.672222222222221</v>
       </c>
     </row>
@@ -3633,10 +3468,10 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D122" s="1">
         <v>19</v>
@@ -3644,7 +3479,7 @@
       <c r="E122" s="1">
         <v>19</v>
       </c>
-      <c r="F122" s="6">
+      <c r="F122" s="2">
         <v>25.230555555555554</v>
       </c>
     </row>
@@ -3656,7 +3491,7 @@
         <v>46</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D123" s="1">
         <v>35</v>
@@ -3664,7 +3499,7 @@
       <c r="E123" s="1">
         <v>19</v>
       </c>
-      <c r="F123" s="6">
+      <c r="F123" s="2">
         <v>30.663888888888888</v>
       </c>
     </row>
@@ -3673,10 +3508,10 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D124" s="1">
         <v>36</v>
@@ -3684,7 +3519,7 @@
       <c r="E124" s="1">
         <v>19</v>
       </c>
-      <c r="F124" s="6">
+      <c r="F124" s="2">
         <v>24.127777777777776</v>
       </c>
     </row>
@@ -3693,10 +3528,10 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D125" s="1">
         <v>37</v>
@@ -3704,7 +3539,7 @@
       <c r="E125" s="1">
         <v>19</v>
       </c>
-      <c r="F125" s="6">
+      <c r="F125" s="2">
         <v>23.022222222222222</v>
       </c>
     </row>
@@ -3713,10 +3548,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D126" s="1">
         <v>38</v>
@@ -3724,7 +3559,7 @@
       <c r="E126" s="1">
         <v>19</v>
       </c>
-      <c r="F126" s="6">
+      <c r="F126" s="2">
         <v>20.880555555555556</v>
       </c>
     </row>
@@ -3736,7 +3571,7 @@
         <v>44</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D127" s="1">
         <v>39</v>
@@ -3744,7 +3579,7 @@
       <c r="E127" s="1">
         <v>19</v>
       </c>
-      <c r="F127" s="6">
+      <c r="F127" s="2">
         <v>26.513888888888889</v>
       </c>
     </row>
@@ -3753,10 +3588,10 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D128" s="1">
         <v>40</v>
@@ -3764,7 +3599,7 @@
       <c r="E128" s="1">
         <v>20</v>
       </c>
-      <c r="F128" s="6">
+      <c r="F128" s="2">
         <v>21.530555555555555</v>
       </c>
     </row>
@@ -3773,10 +3608,10 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D129" s="1">
         <v>41</v>
@@ -3784,7 +3619,7 @@
       <c r="E129" s="1">
         <v>20</v>
       </c>
-      <c r="F129" s="6">
+      <c r="F129" s="2">
         <v>21.56388888888889</v>
       </c>
     </row>
@@ -3793,10 +3628,10 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D130" s="1">
         <v>42</v>
@@ -3804,7 +3639,7 @@
       <c r="E130" s="1">
         <v>20</v>
       </c>
-      <c r="F130" s="6">
+      <c r="F130" s="2">
         <v>23.919444444444444</v>
       </c>
     </row>
@@ -3813,10 +3648,10 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D131" s="1">
         <v>20</v>
@@ -3824,7 +3659,7 @@
       <c r="E131" s="1">
         <v>20</v>
       </c>
-      <c r="F131" s="6">
+      <c r="F131" s="2">
         <v>24.016666666666666</v>
       </c>
     </row>
@@ -3836,7 +3671,7 @@
         <v>14</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D132" s="1">
         <v>60</v>
@@ -3844,7 +3679,7 @@
       <c r="E132" s="1">
         <v>21</v>
       </c>
-      <c r="F132" s="6">
+      <c r="F132" s="2">
         <v>32.12777777777778</v>
       </c>
     </row>
@@ -3856,7 +3691,7 @@
         <v>30</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D133" s="1">
         <v>10</v>
@@ -3864,7 +3699,7 @@
       <c r="E133" s="1">
         <v>21</v>
       </c>
-      <c r="F133" s="6">
+      <c r="F133" s="2">
         <v>29.902777777777779</v>
       </c>
     </row>
@@ -3876,7 +3711,7 @@
         <v>52</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D134" s="1">
         <v>21</v>
@@ -3884,7 +3719,7 @@
       <c r="E134" s="1">
         <v>21</v>
       </c>
-      <c r="F134" s="6">
+      <c r="F134" s="2">
         <v>32.005555555555553</v>
       </c>
     </row>
@@ -3896,7 +3731,7 @@
         <v>66</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D135" s="1">
         <v>11</v>
@@ -3904,7 +3739,7 @@
       <c r="E135" s="1">
         <v>21</v>
       </c>
-      <c r="F135" s="6">
+      <c r="F135" s="2">
         <v>29.058333333333334</v>
       </c>
     </row>
@@ -3913,10 +3748,10 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D136" s="1">
         <v>61</v>
@@ -3924,7 +3759,7 @@
       <c r="E136" s="1">
         <v>21</v>
       </c>
-      <c r="F136" s="6">
+      <c r="F136" s="2">
         <v>25.283333333333335</v>
       </c>
     </row>
@@ -3933,10 +3768,10 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D137" s="1">
         <v>62</v>
@@ -3944,7 +3779,7 @@
       <c r="E137" s="1">
         <v>21</v>
       </c>
-      <c r="F137" s="6">
+      <c r="F137" s="2">
         <v>23.65</v>
       </c>
     </row>
@@ -3953,10 +3788,10 @@
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D138" s="1">
         <v>63</v>
@@ -3964,7 +3799,7 @@
       <c r="E138" s="1">
         <v>21</v>
       </c>
-      <c r="F138" s="6">
+      <c r="F138" s="2">
         <v>24.505555555555556</v>
       </c>
     </row>
@@ -3976,7 +3811,7 @@
         <v>65</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D139" s="1">
         <v>12</v>
@@ -3984,7 +3819,7 @@
       <c r="E139" s="1">
         <v>22</v>
       </c>
-      <c r="F139" s="6">
+      <c r="F139" s="2">
         <v>30.913888888888888</v>
       </c>
     </row>
@@ -3993,10 +3828,10 @@
         <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D140" s="1">
         <v>43</v>
@@ -4004,7 +3839,7 @@
       <c r="E140" s="1">
         <v>22</v>
       </c>
-      <c r="F140" s="6">
+      <c r="F140" s="2">
         <v>26.358333333333334</v>
       </c>
     </row>
@@ -4013,10 +3848,10 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D141" s="1">
         <v>13</v>
@@ -4024,7 +3859,7 @@
       <c r="E141" s="1">
         <v>22</v>
       </c>
-      <c r="F141" s="6">
+      <c r="F141" s="2">
         <v>25.286111111111111</v>
       </c>
     </row>
@@ -4033,10 +3868,10 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D142" s="1">
         <v>14</v>
@@ -4044,7 +3879,7 @@
       <c r="E142" s="1">
         <v>22</v>
       </c>
-      <c r="F142" s="6">
+      <c r="F142" s="2">
         <v>22.483333333333334</v>
       </c>
     </row>
@@ -4053,10 +3888,10 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D143" s="1">
         <v>15</v>
@@ -4064,7 +3899,7 @@
       <c r="E143" s="1">
         <v>22</v>
       </c>
-      <c r="F143" s="6">
+      <c r="F143" s="2">
         <v>22.322222222222223</v>
       </c>
     </row>
@@ -4073,10 +3908,10 @@
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D144" s="1">
         <v>44</v>
@@ -4084,7 +3919,7 @@
       <c r="E144" s="1">
         <v>22</v>
       </c>
-      <c r="F144" s="6">
+      <c r="F144" s="2">
         <v>22.333333333333332</v>
       </c>
     </row>
@@ -4093,10 +3928,10 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D145" s="1">
         <v>45</v>
@@ -4104,7 +3939,7 @@
       <c r="E145" s="1">
         <v>22</v>
       </c>
-      <c r="F145" s="6">
+      <c r="F145" s="2">
         <v>25.091666666666665</v>
       </c>
     </row>
@@ -4113,10 +3948,10 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D146" s="1">
         <v>16</v>
@@ -4124,7 +3959,7 @@
       <c r="E146" s="1">
         <v>22</v>
       </c>
-      <c r="F146" s="6">
+      <c r="F146" s="2">
         <v>26.536111111111111</v>
       </c>
     </row>
@@ -4133,10 +3968,10 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D147" s="1">
         <v>17</v>
@@ -4144,7 +3979,7 @@
       <c r="E147" s="1">
         <v>22</v>
       </c>
-      <c r="F147" s="6">
+      <c r="F147" s="2">
         <v>21.230555555555554</v>
       </c>
     </row>
@@ -4156,7 +3991,7 @@
         <v>13</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D148" s="1">
         <v>18</v>
@@ -4164,7 +3999,7 @@
       <c r="E148" s="1">
         <v>22</v>
       </c>
-      <c r="F148" s="6">
+      <c r="F148" s="2">
         <v>24.819444444444443</v>
       </c>
     </row>
@@ -4173,10 +4008,10 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D149" s="1">
         <v>46</v>
@@ -4184,7 +4019,7 @@
       <c r="E149" s="1">
         <v>22</v>
       </c>
-      <c r="F149" s="6">
+      <c r="F149" s="2">
         <v>25.722222222222221</v>
       </c>
     </row>
@@ -4196,7 +4031,7 @@
         <v>20</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D150" s="1">
         <v>47</v>
@@ -4204,7 +4039,7 @@
       <c r="E150" s="1">
         <v>23</v>
       </c>
-      <c r="F150" s="6">
+      <c r="F150" s="2">
         <v>25.266666666666666</v>
       </c>
     </row>
@@ -4213,10 +4048,10 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D151" s="1">
         <v>48</v>
@@ -4224,7 +4059,7 @@
       <c r="E151" s="1">
         <v>23</v>
       </c>
-      <c r="F151" s="6">
+      <c r="F151" s="2">
         <v>26.552777777777777</v>
       </c>
     </row>
@@ -4233,10 +4068,10 @@
         <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D152" s="1">
         <v>64</v>
@@ -4244,7 +4079,7 @@
       <c r="E152" s="1">
         <v>23</v>
       </c>
-      <c r="F152" s="6">
+      <c r="F152" s="2">
         <v>22.641666666666666</v>
       </c>
     </row>
@@ -4253,10 +4088,10 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D153" s="1">
         <v>22</v>
@@ -4264,7 +4099,7 @@
       <c r="E153" s="1">
         <v>23</v>
       </c>
-      <c r="F153" s="6">
+      <c r="F153" s="2">
         <v>26.405555555555555</v>
       </c>
     </row>
@@ -4276,7 +4111,7 @@
         <v>59</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D154" s="1">
         <v>49</v>
@@ -4284,7 +4119,7 @@
       <c r="E154" s="1">
         <v>23</v>
       </c>
-      <c r="F154" s="6">
+      <c r="F154" s="2">
         <v>27.43888888888889</v>
       </c>
     </row>
@@ -4296,7 +4131,7 @@
         <v>18</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D155" s="1">
         <v>50</v>
@@ -4304,7 +4139,7 @@
       <c r="E155" s="1">
         <v>23</v>
       </c>
-      <c r="F155" s="6">
+      <c r="F155" s="2">
         <v>27.394444444444446</v>
       </c>
     </row>
@@ -4313,10 +4148,10 @@
         <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D156" s="1">
         <v>23</v>
@@ -4324,7 +4159,7 @@
       <c r="E156" s="1">
         <v>23</v>
       </c>
-      <c r="F156" s="6">
+      <c r="F156" s="2">
         <v>23.191666666666666</v>
       </c>
     </row>
@@ -4333,10 +4168,10 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D157" s="1">
         <v>51</v>
@@ -4344,7 +4179,7 @@
       <c r="E157" s="1">
         <v>23</v>
       </c>
-      <c r="F157" s="6">
+      <c r="F157" s="2">
         <v>26.622222222222224</v>
       </c>
     </row>
@@ -4353,10 +4188,10 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D158" s="1">
         <v>24</v>
@@ -4364,7 +4199,7 @@
       <c r="E158" s="1">
         <v>23</v>
       </c>
-      <c r="F158" s="6">
+      <c r="F158" s="2">
         <v>30.797222222222221</v>
       </c>
     </row>
@@ -4373,10 +4208,10 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D159" s="1">
         <v>65</v>
@@ -4384,7 +4219,7 @@
       <c r="E159" s="1">
         <v>23</v>
       </c>
-      <c r="F159" s="6">
+      <c r="F159" s="2">
         <v>24.583333333333332</v>
       </c>
     </row>
@@ -4396,7 +4231,7 @@
         <v>58</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D160" s="1">
         <v>66</v>
@@ -4404,7 +4239,7 @@
       <c r="E160" s="1">
         <v>24</v>
       </c>
-      <c r="F160" s="6">
+      <c r="F160" s="2">
         <v>28.702777777777779</v>
       </c>
     </row>
@@ -4413,10 +4248,10 @@
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D161" s="1">
         <v>67</v>
@@ -4424,7 +4259,7 @@
       <c r="E161" s="1">
         <v>24</v>
       </c>
-      <c r="F161" s="6">
+      <c r="F161" s="2">
         <v>25.672222222222221</v>
       </c>
     </row>
@@ -4433,10 +4268,10 @@
         <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D162" s="1">
         <v>52</v>
@@ -4444,7 +4279,7 @@
       <c r="E162" s="1">
         <v>24</v>
       </c>
-      <c r="F162" s="6">
+      <c r="F162" s="2">
         <v>22.277777777777779</v>
       </c>
     </row>
@@ -4456,7 +4291,7 @@
         <v>64</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D163" s="1">
         <v>25</v>
@@ -4464,7 +4299,7 @@
       <c r="E163" s="1">
         <v>24</v>
       </c>
-      <c r="F163" s="6">
+      <c r="F163" s="2">
         <v>27.413888888888888</v>
       </c>
     </row>
@@ -4473,10 +4308,10 @@
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D164" s="1">
         <v>26</v>
@@ -4484,7 +4319,7 @@
       <c r="E164" s="1">
         <v>24</v>
       </c>
-      <c r="F164" s="6">
+      <c r="F164" s="2">
         <v>22.216666666666665</v>
       </c>
     </row>
@@ -4496,7 +4331,7 @@
         <v>38</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D165" s="1">
         <v>19</v>
@@ -4504,7 +4339,7 @@
       <c r="E165" s="1">
         <v>24</v>
       </c>
-      <c r="F165" s="6">
+      <c r="F165" s="2">
         <v>35.822222222222223</v>
       </c>
     </row>
@@ -4513,10 +4348,10 @@
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D166" s="1">
         <v>53</v>
@@ -4524,7 +4359,7 @@
       <c r="E166" s="1">
         <v>25</v>
       </c>
-      <c r="F166" s="6">
+      <c r="F166" s="2">
         <v>22.588888888888889</v>
       </c>
     </row>
@@ -4533,10 +4368,10 @@
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D167" s="1">
         <v>54</v>
@@ -4544,7 +4379,7 @@
       <c r="E167" s="1">
         <v>25</v>
       </c>
-      <c r="F167" s="6">
+      <c r="F167" s="2">
         <v>21.930555555555557</v>
       </c>
     </row>
@@ -4553,10 +4388,10 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D168" s="1">
         <v>68</v>
@@ -4564,7 +4399,7 @@
       <c r="E168" s="1">
         <v>25</v>
       </c>
-      <c r="F168" s="6">
+      <c r="F168" s="2">
         <v>22.452777777777779</v>
       </c>
     </row>
@@ -4573,10 +4408,10 @@
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D169" s="1">
         <v>69</v>
@@ -4584,7 +4419,7 @@
       <c r="E169" s="1">
         <v>25</v>
       </c>
-      <c r="F169" s="6">
+      <c r="F169" s="2">
         <v>22.81388888888889</v>
       </c>
     </row>
@@ -4593,10 +4428,10 @@
         <v>169</v>
       </c>
       <c r="B170" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D170" s="1">
         <v>70</v>
@@ -4604,7 +4439,7 @@
       <c r="E170" s="1">
         <v>25</v>
       </c>
-      <c r="F170" s="6">
+      <c r="F170" s="2">
         <v>25.3</v>
       </c>
     </row>
@@ -4613,10 +4448,10 @@
         <v>170</v>
       </c>
       <c r="B171" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D171" s="1">
         <v>20</v>
@@ -4624,7 +4459,7 @@
       <c r="E171" s="1">
         <v>25</v>
       </c>
-      <c r="F171" s="6">
+      <c r="F171" s="2">
         <v>24.594444444444445</v>
       </c>
     </row>
@@ -4633,10 +4468,10 @@
         <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D172" s="1">
         <v>21</v>
@@ -4644,7 +4479,7 @@
       <c r="E172" s="1">
         <v>25</v>
       </c>
-      <c r="F172" s="6">
+      <c r="F172" s="2">
         <v>21.030555555555555</v>
       </c>
     </row>
@@ -4653,10 +4488,10 @@
         <v>172</v>
       </c>
       <c r="B173" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D173" s="1">
         <v>22</v>
@@ -4664,7 +4499,7 @@
       <c r="E173" s="1">
         <v>25</v>
       </c>
-      <c r="F173" s="6">
+      <c r="F173" s="2">
         <v>29.941666666666666</v>
       </c>
     </row>
@@ -4673,10 +4508,10 @@
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D174" s="1">
         <v>71</v>
@@ -4684,7 +4519,7 @@
       <c r="E174" s="1">
         <v>26</v>
       </c>
-      <c r="F174" s="6">
+      <c r="F174" s="2">
         <v>23.752777777777776</v>
       </c>
     </row>
@@ -4693,10 +4528,10 @@
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D175" s="1">
         <v>55</v>
@@ -4704,7 +4539,7 @@
       <c r="E175" s="1">
         <v>26</v>
       </c>
-      <c r="F175" s="6">
+      <c r="F175" s="2">
         <v>22.027777777777779</v>
       </c>
     </row>
@@ -4713,10 +4548,10 @@
         <v>175</v>
       </c>
       <c r="B176" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D176" s="1">
         <v>56</v>
@@ -4724,7 +4559,7 @@
       <c r="E176" s="1">
         <v>26</v>
       </c>
-      <c r="F176" s="6">
+      <c r="F176" s="2">
         <v>25.886111111111113</v>
       </c>
     </row>
@@ -4733,10 +4568,10 @@
         <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D177" s="1">
         <v>72</v>
@@ -4744,7 +4579,7 @@
       <c r="E177" s="1">
         <v>26</v>
       </c>
-      <c r="F177" s="6">
+      <c r="F177" s="2">
         <v>28.158333333333335</v>
       </c>
     </row>
@@ -4753,10 +4588,10 @@
         <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D178" s="1">
         <v>57</v>
@@ -4764,7 +4599,7 @@
       <c r="E178" s="1">
         <v>26</v>
       </c>
-      <c r="F178" s="6">
+      <c r="F178" s="2">
         <v>24.502777777777776</v>
       </c>
     </row>
@@ -4776,7 +4611,7 @@
         <v>54</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D179" s="1">
         <v>23</v>
@@ -4784,7 +4619,7 @@
       <c r="E179" s="1">
         <v>26</v>
       </c>
-      <c r="F179" s="6">
+      <c r="F179" s="2">
         <v>30.577777777777779</v>
       </c>
     </row>
@@ -4793,10 +4628,10 @@
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D180" s="1">
         <v>58</v>
@@ -4804,7 +4639,7 @@
       <c r="E180" s="1">
         <v>26</v>
       </c>
-      <c r="F180" s="6">
+      <c r="F180" s="2">
         <v>25.294444444444444</v>
       </c>
     </row>
@@ -4813,10 +4648,10 @@
         <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D181" s="1">
         <v>73</v>
@@ -4824,7 +4659,7 @@
       <c r="E181" s="1">
         <v>26</v>
       </c>
-      <c r="F181" s="6">
+      <c r="F181" s="2">
         <v>26.219444444444445</v>
       </c>
     </row>
@@ -4836,7 +4671,7 @@
         <v>55</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D182" s="1">
         <v>24</v>
@@ -4844,7 +4679,7 @@
       <c r="E182" s="1">
         <v>26</v>
       </c>
-      <c r="F182" s="6">
+      <c r="F182" s="2">
         <v>26.766666666666666</v>
       </c>
     </row>
@@ -4853,10 +4688,10 @@
         <v>182</v>
       </c>
       <c r="B183" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D183" s="1">
         <v>59</v>
@@ -4864,7 +4699,7 @@
       <c r="E183" s="1">
         <v>26</v>
       </c>
-      <c r="F183" s="6">
+      <c r="F183" s="2">
         <v>24.588888888888889</v>
       </c>
     </row>
@@ -4873,10 +4708,10 @@
         <v>183</v>
       </c>
       <c r="B184" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D184" s="1">
         <v>60</v>
@@ -4884,7 +4719,7 @@
       <c r="E184" s="1">
         <v>26</v>
       </c>
-      <c r="F184" s="6">
+      <c r="F184" s="2">
         <v>27.130555555555556</v>
       </c>
     </row>
@@ -4893,10 +4728,10 @@
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D185" s="1">
         <v>74</v>
@@ -4904,7 +4739,7 @@
       <c r="E185" s="1">
         <v>27</v>
       </c>
-      <c r="F185" s="6">
+      <c r="F185" s="2">
         <v>23.005555555555556</v>
       </c>
     </row>
@@ -4913,10 +4748,10 @@
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D186" s="1">
         <v>61</v>
@@ -4924,7 +4759,7 @@
       <c r="E186" s="1">
         <v>27</v>
       </c>
-      <c r="F186" s="6">
+      <c r="F186" s="2">
         <v>0</v>
       </c>
     </row>
@@ -4933,10 +4768,10 @@
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D187" s="1">
         <v>62</v>
@@ -4944,7 +4779,7 @@
       <c r="E187" s="1">
         <v>27</v>
       </c>
-      <c r="F187" s="6">
+      <c r="F187" s="2">
         <v>21.969444444444445</v>
       </c>
     </row>
@@ -4953,10 +4788,10 @@
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D188" s="1">
         <v>75</v>
@@ -4964,7 +4799,7 @@
       <c r="E188" s="1">
         <v>27</v>
       </c>
-      <c r="F188" s="6">
+      <c r="F188" s="2">
         <v>22.669444444444444</v>
       </c>
     </row>
@@ -4973,10 +4808,10 @@
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D189" s="1">
         <v>76</v>
@@ -4984,7 +4819,7 @@
       <c r="E189" s="1">
         <v>28</v>
       </c>
-      <c r="F189" s="6">
+      <c r="F189" s="2">
         <v>22.127777777777776</v>
       </c>
     </row>
@@ -4993,10 +4828,10 @@
         <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D190" s="1">
         <v>63</v>
@@ -5004,7 +4839,7 @@
       <c r="E190" s="1">
         <v>28</v>
       </c>
-      <c r="F190" s="6">
+      <c r="F190" s="2">
         <v>23.377777777777776</v>
       </c>
     </row>
@@ -5013,10 +4848,10 @@
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D191" s="1">
         <v>25</v>
@@ -5024,7 +4859,7 @@
       <c r="E191" s="1">
         <v>28</v>
       </c>
-      <c r="F191" s="6">
+      <c r="F191" s="2">
         <v>22.344444444444445</v>
       </c>
     </row>
@@ -5033,10 +4868,10 @@
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D192" s="1">
         <v>26</v>
@@ -5044,7 +4879,7 @@
       <c r="E192" s="1">
         <v>28</v>
       </c>
-      <c r="F192" s="6">
+      <c r="F192" s="2">
         <v>24.430555555555557</v>
       </c>
     </row>
@@ -5053,10 +4888,10 @@
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D193" s="1">
         <v>64</v>
@@ -5064,7 +4899,7 @@
       <c r="E193" s="1">
         <v>28</v>
       </c>
-      <c r="F193" s="6">
+      <c r="F193" s="2">
         <v>24.683333333333334</v>
       </c>
     </row>
@@ -5073,10 +4908,10 @@
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D194" s="1">
         <v>27</v>
@@ -5084,7 +4919,7 @@
       <c r="E194" s="1">
         <v>28</v>
       </c>
-      <c r="F194" s="6">
+      <c r="F194" s="2">
         <v>22.1</v>
       </c>
     </row>
@@ -5093,10 +4928,10 @@
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D195" s="1">
         <v>77</v>
@@ -5104,7 +4939,7 @@
       <c r="E195" s="1">
         <v>29</v>
       </c>
-      <c r="F195" s="6">
+      <c r="F195" s="2">
         <v>24.125</v>
       </c>
     </row>
@@ -5113,10 +4948,10 @@
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D196" s="1">
         <v>28</v>
@@ -5124,7 +4959,7 @@
       <c r="E196" s="1">
         <v>29</v>
       </c>
-      <c r="F196" s="6">
+      <c r="F196" s="2">
         <v>26.252777777777776</v>
       </c>
     </row>
@@ -5133,10 +4968,10 @@
         <v>196</v>
       </c>
       <c r="B197" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D197" s="1">
         <v>78</v>
@@ -5144,7 +4979,7 @@
       <c r="E197" s="1">
         <v>29</v>
       </c>
-      <c r="F197" s="6">
+      <c r="F197" s="2">
         <v>24.572222222222223</v>
       </c>
     </row>
@@ -5153,10 +4988,10 @@
         <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D198" s="1">
         <v>79</v>
@@ -5164,7 +4999,7 @@
       <c r="E198" s="1">
         <v>29</v>
       </c>
-      <c r="F198" s="6">
+      <c r="F198" s="2">
         <v>25.858333333333334</v>
       </c>
     </row>
@@ -5173,10 +5008,10 @@
         <v>198</v>
       </c>
       <c r="B199" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D199" s="1">
         <v>80</v>
@@ -5184,7 +5019,7 @@
       <c r="E199" s="1">
         <v>30</v>
       </c>
-      <c r="F199" s="6">
+      <c r="F199" s="2">
         <v>25.755555555555556</v>
       </c>
     </row>
@@ -5193,10 +5028,10 @@
         <v>199</v>
       </c>
       <c r="B200" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D200" s="1">
         <v>81</v>
@@ -5204,7 +5039,7 @@
       <c r="E200" s="1">
         <v>30</v>
       </c>
-      <c r="F200" s="6">
+      <c r="F200" s="2">
         <v>23.225000000000001</v>
       </c>
     </row>
@@ -5213,10 +5048,10 @@
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D201" s="1">
         <v>65</v>
@@ -5224,7 +5059,7 @@
       <c r="E201" s="1">
         <v>30</v>
       </c>
-      <c r="F201" s="6">
+      <c r="F201" s="2">
         <v>23.216666666666665</v>
       </c>
     </row>

</xml_diff>